<commit_message>
wip: added module for allocations check
</commit_message>
<xml_diff>
--- a/tests/resources/test_plan.xlsx
+++ b/tests/resources/test_plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PP\ganttly\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988225C4-EF93-488D-9AA2-E358C44FF4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1A5921-8DA4-4184-9528-987BEB6974FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C855B014-DAAA-4E56-AA0D-6682439151A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{C855B014-DAAA-4E56-AA0D-6682439151A2}"/>
   </bookViews>
   <sheets>
     <sheet name="MyPlan" sheetId="4" r:id="rId1"/>
+    <sheet name="Allocations" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Start Date</t>
   </si>
@@ -88,6 +89,57 @@
   </si>
   <si>
     <t>AFU</t>
+  </si>
+  <si>
+    <t>Persone</t>
+  </si>
+  <si>
+    <t>Attività</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>Mese-Anno</t>
+  </si>
+  <si>
+    <t>Anno</t>
+  </si>
+  <si>
+    <t>Giornate</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Check Allocazione Nel Piano</t>
+  </si>
+  <si>
+    <t>Requisiti di Accesso - M_Mutui_ATE_Task</t>
+  </si>
+  <si>
+    <t>Requisiti di Accesso - M</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Requisiti di Accesso - M_Mutui_AFU_Task</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Emanuelo</t>
+  </si>
+  <si>
+    <t>Vittoriana</t>
+  </si>
+  <si>
+    <t>Stream 2</t>
+  </si>
+  <si>
+    <t>Stream 2 - Sviluppi</t>
   </si>
 </sst>
 </file>
@@ -147,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,11 +208,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -472,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A252246-3B78-4B49-9CAE-3153B0DA4C82}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -649,6 +726,175 @@
       <c r="F9" s="1"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55C9132-D4BF-4323-AD42-99502EDD399F}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5">
+        <v>45536</v>
+      </c>
+      <c r="F2">
+        <v>2024</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="5">
+        <v>45536</v>
+      </c>
+      <c r="K2" s="5">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5">
+        <v>45536</v>
+      </c>
+      <c r="F3">
+        <v>2024</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="5">
+        <v>45550</v>
+      </c>
+      <c r="K3" s="5">
+        <v>45600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5">
+        <v>45505</v>
+      </c>
+      <c r="F4">
+        <v>2024</v>
+      </c>
+      <c r="G4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5">
+        <v>45512</v>
+      </c>
+      <c r="K4" s="5">
+        <v>45536</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H1:K1">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>NETWORKDAYS(EOMONTH(G1, -1) + 1, EOMONTH(G1, 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>NETWORKDAYS(EOMONTH(E1, -1) + 1, EOMONTH(E1, 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -798,18 +1044,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -831,18 +1077,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E970455-BE7B-4D93-AB4F-90D1DB26222C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBB22C7A-415F-456C-B5C1-B54A6C14B9A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E970455-BE7B-4D93-AB4F-90D1DB26222C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>